<commit_message>
synthetic experiment results updated
</commit_message>
<xml_diff>
--- a/data/synthetic_exp_results.xlsx
+++ b/data/synthetic_exp_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1663,6 +1663,402 @@
         <v>0.9046595512093797</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>LGBM Baseline</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.565989847715736</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.565989847715736</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.9968309859154929</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.9968309859154929</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.9981804369560553</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.9981804369560553</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>LGBM Upsample</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.1715260545905707</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.9748037512393462</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.9505003706449222</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.9742003986364398</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.994321693648723</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.9943616762474357</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>LGBM Downsample</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.03798162621692033</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.7399555226093403</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.9711692506168886</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>SMOTE LGBM</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.07346881765486417</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.9143096339772789</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.8770663454410674</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.9113406478773541</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.9708859657552483</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.9692645787690264</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>LGBM Balanced Bagging</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.3777452415812592</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.3777452415812592</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.9960618977020015</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.9960618977020015</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.9999730501107887</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.9999730501107887</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>LGBM_Imbalance</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0954427433073686</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.0954427433073686</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.9063843587842847</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.9063843587842847</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.9576621527591677</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.9576621527591677</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>LGBM Baseline</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.5572916666666667</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.9947741002927987</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.9968495181616012</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.7856255670059564</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.9989981110762746</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>LGBM Upsample</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0648854961832061</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.9742856752684549</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.945517215818539</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.9736942592109675</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.8444959591937506</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.9939958935087631</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>LGBM Downsample</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.02641408751334045</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.729513361254216</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.8133324028620204</v>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>SMOTE LGBM</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.04306350504224585</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.9065770245264153</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.8698713909788369</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.9038436463882576</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.8431981862846573</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.9655339671578294</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>LGBM Balanced Bagging</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.4069767441860465</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.9952929839516697</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.9962194217939214</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.8249686698971221</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.9999287727692603</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Synthetic-0.5</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>LGBM_Imbalance</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.02310924369747899</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.05368421052631579</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.8621251992142619</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.8667160859896219</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.6034083985200814</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.8793823951574593</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>